<commit_message>
added new variables (dist. travelled from 15-30 min) + update some plots
</commit_message>
<xml_diff>
--- a/summary_tracking.xlsx
+++ b/summary_tracking.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE78"/>
+  <dimension ref="A1:AH78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -513,6 +513,21 @@
           <t>dist_trav_15min_body_out</t>
         </is>
       </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>dist_trav_20min_body_out</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>dist_trav_25min_body_out</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>dist_trav_30min_body_out</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -608,6 +623,15 @@
       <c r="AE2">
         <v>0</v>
       </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3">
@@ -703,6 +727,15 @@
       <c r="AE3">
         <v>0</v>
       </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4">
@@ -798,6 +831,15 @@
       <c r="AE4">
         <v>23.1612218944</v>
       </c>
+      <c r="AF4">
+        <v>29.065045753</v>
+      </c>
+      <c r="AG4">
+        <v>43.707970517</v>
+      </c>
+      <c r="AH4">
+        <v>53.959036928</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5">
@@ -893,6 +935,15 @@
       <c r="AE5">
         <v>37.7508218761</v>
       </c>
+      <c r="AF5">
+        <v>51.8091856353</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -988,6 +1039,15 @@
       <c r="AE6">
         <v>51.2659130981</v>
       </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7">
@@ -1083,6 +1143,15 @@
       <c r="AE7">
         <v>0</v>
       </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
+        <v>0</v>
+      </c>
+      <c r="AH7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8">
@@ -1178,6 +1247,15 @@
       <c r="AE8">
         <v>0</v>
       </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9">
@@ -1273,6 +1351,15 @@
       <c r="AE9">
         <v>0</v>
       </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>0</v>
+      </c>
+      <c r="AH9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10">
@@ -1368,6 +1455,15 @@
       <c r="AE10">
         <v>76.996396233</v>
       </c>
+      <c r="AF10">
+        <v>97.496614224</v>
+      </c>
+      <c r="AG10">
+        <v>116.082207546</v>
+      </c>
+      <c r="AH10">
+        <v>134.850822292</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11">
@@ -1463,6 +1559,15 @@
       <c r="AE11">
         <v>0</v>
       </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12">
@@ -1558,6 +1663,15 @@
       <c r="AE12">
         <v>0</v>
       </c>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12">
+        <v>0</v>
+      </c>
+      <c r="AH12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13">
@@ -1653,6 +1767,15 @@
       <c r="AE13">
         <v>38.5110019221</v>
       </c>
+      <c r="AF13">
+        <v>55.8808590596</v>
+      </c>
+      <c r="AG13">
+        <v>69.97903018229999</v>
+      </c>
+      <c r="AH13">
+        <v>87.1682587289</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14">
@@ -1748,6 +1871,15 @@
       <c r="AE14">
         <v>0</v>
       </c>
+      <c r="AF14">
+        <v>0</v>
+      </c>
+      <c r="AG14">
+        <v>0</v>
+      </c>
+      <c r="AH14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15">
@@ -1843,6 +1975,15 @@
       <c r="AE15">
         <v>0</v>
       </c>
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15">
+        <v>0</v>
+      </c>
+      <c r="AH15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16">
@@ -1938,6 +2079,15 @@
       <c r="AE16">
         <v>0</v>
       </c>
+      <c r="AF16">
+        <v>0</v>
+      </c>
+      <c r="AG16">
+        <v>0</v>
+      </c>
+      <c r="AH16">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17">
@@ -2033,6 +2183,15 @@
       <c r="AE17">
         <v>49.7084271884</v>
       </c>
+      <c r="AF17">
+        <v>71.51811290969999</v>
+      </c>
+      <c r="AG17">
+        <v>83.4898792445</v>
+      </c>
+      <c r="AH17">
+        <v>94.83043631629999</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18">
@@ -2128,6 +2287,15 @@
       <c r="AE18">
         <v>60.545914894</v>
       </c>
+      <c r="AF18">
+        <v>74.51979790576</v>
+      </c>
+      <c r="AG18">
+        <v>86.63974060347</v>
+      </c>
+      <c r="AH18">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19">
@@ -2223,6 +2391,15 @@
       <c r="AE19">
         <v>0</v>
       </c>
+      <c r="AF19">
+        <v>0</v>
+      </c>
+      <c r="AG19">
+        <v>0</v>
+      </c>
+      <c r="AH19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20">
@@ -2318,6 +2495,15 @@
       <c r="AE20">
         <v>0</v>
       </c>
+      <c r="AF20">
+        <v>0</v>
+      </c>
+      <c r="AG20">
+        <v>0</v>
+      </c>
+      <c r="AH20">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21">
@@ -2413,6 +2599,15 @@
       <c r="AE21">
         <v>0</v>
       </c>
+      <c r="AF21">
+        <v>0</v>
+      </c>
+      <c r="AG21">
+        <v>0</v>
+      </c>
+      <c r="AH21">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22">
@@ -2508,6 +2703,15 @@
       <c r="AE22">
         <v>46.765308828</v>
       </c>
+      <c r="AF22">
+        <v>60.851160999</v>
+      </c>
+      <c r="AG22">
+        <v>75.42470776499999</v>
+      </c>
+      <c r="AH22">
+        <v>85.755232096</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23">
@@ -2603,6 +2807,15 @@
       <c r="AE23">
         <v>88.28189068</v>
       </c>
+      <c r="AF23">
+        <v>113.053870372</v>
+      </c>
+      <c r="AG23">
+        <v>136.9123724667</v>
+      </c>
+      <c r="AH23">
+        <v>156.0485786097</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24">
@@ -2698,6 +2911,15 @@
       <c r="AE24">
         <v>59.18477003</v>
       </c>
+      <c r="AF24">
+        <v>75.196236946</v>
+      </c>
+      <c r="AG24">
+        <v>89.062112793</v>
+      </c>
+      <c r="AH24">
+        <v>106.651700849</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25">
@@ -2793,6 +3015,15 @@
       <c r="AE25">
         <v>0</v>
       </c>
+      <c r="AF25">
+        <v>0</v>
+      </c>
+      <c r="AG25">
+        <v>0</v>
+      </c>
+      <c r="AH25">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26">
@@ -2888,6 +3119,15 @@
       <c r="AE26">
         <v>0</v>
       </c>
+      <c r="AF26">
+        <v>0</v>
+      </c>
+      <c r="AG26">
+        <v>0</v>
+      </c>
+      <c r="AH26">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27">
@@ -2983,6 +3223,15 @@
       <c r="AE27">
         <v>0</v>
       </c>
+      <c r="AF27">
+        <v>0</v>
+      </c>
+      <c r="AG27">
+        <v>0</v>
+      </c>
+      <c r="AH27">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28">
@@ -3078,6 +3327,15 @@
       <c r="AE28">
         <v>59.452279021</v>
       </c>
+      <c r="AF28">
+        <v>75.513032749</v>
+      </c>
+      <c r="AG28">
+        <v>94.486585324</v>
+      </c>
+      <c r="AH28">
+        <v>115.689266338</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29">
@@ -3173,6 +3431,15 @@
       <c r="AE29">
         <v>26.3823350634</v>
       </c>
+      <c r="AF29">
+        <v>43.7300336234</v>
+      </c>
+      <c r="AG29">
+        <v>68.1845941214</v>
+      </c>
+      <c r="AH29">
+        <v>85.9006444444</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30">
@@ -3268,6 +3535,15 @@
       <c r="AE30">
         <v>43.1434960101</v>
       </c>
+      <c r="AF30">
+        <v>57.8923168888</v>
+      </c>
+      <c r="AG30">
+        <v>79.8039617264</v>
+      </c>
+      <c r="AH30">
+        <v>97.59974628339999</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31">
@@ -3363,6 +3639,15 @@
       <c r="AE31">
         <v>60.0486597332</v>
       </c>
+      <c r="AF31">
+        <v>80.48688252620001</v>
+      </c>
+      <c r="AG31">
+        <v>81.5736840917</v>
+      </c>
+      <c r="AH31">
+        <v>83.6186979527</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32">
@@ -3458,6 +3743,15 @@
       <c r="AE32">
         <v>59.797433178</v>
       </c>
+      <c r="AF32">
+        <v>81.55335022200001</v>
+      </c>
+      <c r="AG32">
+        <v>93.657725305</v>
+      </c>
+      <c r="AH32">
+        <v>109.372537696</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33">
@@ -3553,6 +3847,15 @@
       <c r="AE33">
         <v>0</v>
       </c>
+      <c r="AF33">
+        <v>0</v>
+      </c>
+      <c r="AG33">
+        <v>0</v>
+      </c>
+      <c r="AH33">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34">
@@ -3648,6 +3951,15 @@
       <c r="AE34">
         <v>81.866519662</v>
       </c>
+      <c r="AF34">
+        <v>106.71652432</v>
+      </c>
+      <c r="AG34">
+        <v>129.559830121</v>
+      </c>
+      <c r="AH34">
+        <v>155.295083402</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35">
@@ -3743,6 +4055,15 @@
       <c r="AE35">
         <v>35.148505659</v>
       </c>
+      <c r="AF35">
+        <v>0</v>
+      </c>
+      <c r="AG35">
+        <v>0</v>
+      </c>
+      <c r="AH35">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36">
@@ -3838,6 +4159,15 @@
       <c r="AE36">
         <v>86.61321055400001</v>
       </c>
+      <c r="AF36">
+        <v>117.346722634</v>
+      </c>
+      <c r="AG36">
+        <v>134.538752376</v>
+      </c>
+      <c r="AH36">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37">
@@ -3933,6 +4263,15 @@
       <c r="AE37">
         <v>0</v>
       </c>
+      <c r="AF37">
+        <v>0</v>
+      </c>
+      <c r="AG37">
+        <v>0</v>
+      </c>
+      <c r="AH37">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38">
@@ -4028,6 +4367,15 @@
       <c r="AE38">
         <v>60.573625189</v>
       </c>
+      <c r="AF38">
+        <v>82.65475698100001</v>
+      </c>
+      <c r="AG38">
+        <v>107.271065678</v>
+      </c>
+      <c r="AH38">
+        <v>130.592298752</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39">
@@ -4123,6 +4471,15 @@
       <c r="AE39">
         <v>68.43206845820001</v>
       </c>
+      <c r="AF39">
+        <v>91.5006471005</v>
+      </c>
+      <c r="AG39">
+        <v>109.0869068761</v>
+      </c>
+      <c r="AH39">
+        <v>127.5684101063</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40">
@@ -4218,6 +4575,15 @@
       <c r="AE40">
         <v>47.956995273</v>
       </c>
+      <c r="AF40">
+        <v>55.375485867</v>
+      </c>
+      <c r="AG40">
+        <v>55.375485867</v>
+      </c>
+      <c r="AH40">
+        <v>55.375485867</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41">
@@ -4313,6 +4679,15 @@
       <c r="AE41">
         <v>0</v>
       </c>
+      <c r="AF41">
+        <v>0</v>
+      </c>
+      <c r="AG41">
+        <v>0</v>
+      </c>
+      <c r="AH41">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42">
@@ -4408,6 +4783,15 @@
       <c r="AE42">
         <v>60.5111875448</v>
       </c>
+      <c r="AF42">
+        <v>79.102341307</v>
+      </c>
+      <c r="AG42">
+        <v>105.3188281953</v>
+      </c>
+      <c r="AH42">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43">
@@ -4503,6 +4887,15 @@
       <c r="AE43">
         <v>0</v>
       </c>
+      <c r="AF43">
+        <v>0</v>
+      </c>
+      <c r="AG43">
+        <v>0</v>
+      </c>
+      <c r="AH43">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44">
@@ -4598,6 +4991,15 @@
       <c r="AE44">
         <v>55.461370928</v>
       </c>
+      <c r="AF44">
+        <v>71.281038159</v>
+      </c>
+      <c r="AG44">
+        <v>88.412876766</v>
+      </c>
+      <c r="AH44">
+        <v>103.163733472</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45">
@@ -4693,6 +5095,15 @@
       <c r="AE45">
         <v>36.861188311</v>
       </c>
+      <c r="AF45">
+        <v>52.705811749</v>
+      </c>
+      <c r="AG45">
+        <v>63.016966618</v>
+      </c>
+      <c r="AH45">
+        <v>73.402168129</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46">
@@ -4788,6 +5199,15 @@
       <c r="AE46">
         <v>43.202783916</v>
       </c>
+      <c r="AF46">
+        <v>51.872209149</v>
+      </c>
+      <c r="AG46">
+        <v>66.26112639500001</v>
+      </c>
+      <c r="AH46">
+        <v>80.42873317900001</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47">
@@ -4883,6 +5303,15 @@
       <c r="AE47">
         <v>55.654138764</v>
       </c>
+      <c r="AF47">
+        <v>75.556626194</v>
+      </c>
+      <c r="AG47">
+        <v>94.40515643099999</v>
+      </c>
+      <c r="AH47">
+        <v>109.044053422</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48">
@@ -4978,6 +5407,15 @@
       <c r="AE48">
         <v>77.401083298</v>
       </c>
+      <c r="AF48">
+        <v>97.624565797</v>
+      </c>
+      <c r="AG48">
+        <v>113.303162893</v>
+      </c>
+      <c r="AH48">
+        <v>137.560560446</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49">
@@ -5073,6 +5511,15 @@
       <c r="AE49">
         <v>0</v>
       </c>
+      <c r="AF49">
+        <v>0</v>
+      </c>
+      <c r="AG49">
+        <v>0</v>
+      </c>
+      <c r="AH49">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50">
@@ -5168,6 +5615,15 @@
       <c r="AE50">
         <v>57.250328895</v>
       </c>
+      <c r="AF50">
+        <v>72.61480394500001</v>
+      </c>
+      <c r="AG50">
+        <v>0</v>
+      </c>
+      <c r="AH50">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51">
@@ -5263,6 +5719,15 @@
       <c r="AE51">
         <v>56.405327607</v>
       </c>
+      <c r="AF51">
+        <v>60.252062814</v>
+      </c>
+      <c r="AG51">
+        <v>76.023184211</v>
+      </c>
+      <c r="AH51">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52">
@@ -5358,6 +5823,15 @@
       <c r="AE52">
         <v>64.08830491000001</v>
       </c>
+      <c r="AF52">
+        <v>83.365981737</v>
+      </c>
+      <c r="AG52">
+        <v>101.725452821</v>
+      </c>
+      <c r="AH52">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53">
@@ -5453,6 +5927,15 @@
       <c r="AE53">
         <v>49.93025029</v>
       </c>
+      <c r="AF53">
+        <v>71.552019311</v>
+      </c>
+      <c r="AG53">
+        <v>92.298918266</v>
+      </c>
+      <c r="AH53">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54">
@@ -5548,6 +6031,15 @@
       <c r="AE54">
         <v>79.99727161</v>
       </c>
+      <c r="AF54">
+        <v>93.87450332909999</v>
+      </c>
+      <c r="AG54">
+        <v>115.232602715</v>
+      </c>
+      <c r="AH54">
+        <v>128.1463967038</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55">
@@ -5643,6 +6135,15 @@
       <c r="AE55">
         <v>52.99454133</v>
       </c>
+      <c r="AF55">
+        <v>75.85890205699999</v>
+      </c>
+      <c r="AG55">
+        <v>0</v>
+      </c>
+      <c r="AH55">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56">
@@ -5738,6 +6239,15 @@
       <c r="AE56">
         <v>99.85351828</v>
       </c>
+      <c r="AF56">
+        <v>118.687446339</v>
+      </c>
+      <c r="AG56">
+        <v>135.011023018</v>
+      </c>
+      <c r="AH56">
+        <v>151.616284415</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57">
@@ -5833,6 +6343,15 @@
       <c r="AE57">
         <v>0</v>
       </c>
+      <c r="AF57">
+        <v>0</v>
+      </c>
+      <c r="AG57">
+        <v>0</v>
+      </c>
+      <c r="AH57">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58">
@@ -5928,6 +6447,15 @@
       <c r="AE58">
         <v>41.794881063</v>
       </c>
+      <c r="AF58">
+        <v>52.447994867</v>
+      </c>
+      <c r="AG58">
+        <v>0</v>
+      </c>
+      <c r="AH58">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59">
@@ -6023,6 +6551,15 @@
       <c r="AE59">
         <v>65.453929522</v>
       </c>
+      <c r="AF59">
+        <v>85.908890035</v>
+      </c>
+      <c r="AG59">
+        <v>104.010235133</v>
+      </c>
+      <c r="AH59">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60">
@@ -6118,6 +6655,15 @@
       <c r="AE60">
         <v>57.0645241494</v>
       </c>
+      <c r="AF60">
+        <v>0</v>
+      </c>
+      <c r="AG60">
+        <v>0</v>
+      </c>
+      <c r="AH60">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61">
@@ -6213,6 +6759,15 @@
       <c r="AE61">
         <v>53.364162061</v>
       </c>
+      <c r="AF61">
+        <v>0</v>
+      </c>
+      <c r="AG61">
+        <v>0</v>
+      </c>
+      <c r="AH61">
+        <v>0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62">
@@ -6308,6 +6863,15 @@
       <c r="AE62">
         <v>64.41886128500001</v>
       </c>
+      <c r="AF62">
+        <v>85.88790569299999</v>
+      </c>
+      <c r="AG62">
+        <v>95.810562464</v>
+      </c>
+      <c r="AH62">
+        <v>99.15457831800001</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63">
@@ -6403,6 +6967,15 @@
       <c r="AE63">
         <v>55.3156272122</v>
       </c>
+      <c r="AF63">
+        <v>74.8552253232</v>
+      </c>
+      <c r="AG63">
+        <v>91.9242211235</v>
+      </c>
+      <c r="AH63">
+        <v>107.9400711688</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64">
@@ -6498,6 +7071,15 @@
       <c r="AE64">
         <v>0</v>
       </c>
+      <c r="AF64">
+        <v>0</v>
+      </c>
+      <c r="AG64">
+        <v>0</v>
+      </c>
+      <c r="AH64">
+        <v>0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65">
@@ -6593,6 +7175,15 @@
       <c r="AE65">
         <v>40.170302651</v>
       </c>
+      <c r="AF65">
+        <v>58.623882499</v>
+      </c>
+      <c r="AG65">
+        <v>76.571656111</v>
+      </c>
+      <c r="AH65">
+        <v>93.370780098</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66">
@@ -6688,6 +7279,15 @@
       <c r="AE66">
         <v>92.529795609</v>
       </c>
+      <c r="AF66">
+        <v>0</v>
+      </c>
+      <c r="AG66">
+        <v>0</v>
+      </c>
+      <c r="AH66">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67">
@@ -6783,6 +7383,15 @@
       <c r="AE67">
         <v>54.367380646</v>
       </c>
+      <c r="AF67">
+        <v>64.94725393</v>
+      </c>
+      <c r="AG67">
+        <v>80.330597814</v>
+      </c>
+      <c r="AH67">
+        <v>94.596163937</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68">
@@ -6878,6 +7487,15 @@
       <c r="AE68">
         <v>0</v>
       </c>
+      <c r="AF68">
+        <v>0</v>
+      </c>
+      <c r="AG68">
+        <v>0</v>
+      </c>
+      <c r="AH68">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69">
@@ -6973,6 +7591,15 @@
       <c r="AE69">
         <v>95.013650626</v>
       </c>
+      <c r="AF69">
+        <v>127.480112912</v>
+      </c>
+      <c r="AG69">
+        <v>162.091526286</v>
+      </c>
+      <c r="AH69">
+        <v>194.844537196</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70">
@@ -7068,6 +7695,15 @@
       <c r="AE70">
         <v>46.5057401888</v>
       </c>
+      <c r="AF70">
+        <v>70.9797245953</v>
+      </c>
+      <c r="AG70">
+        <v>0</v>
+      </c>
+      <c r="AH70">
+        <v>0</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71">
@@ -7163,6 +7799,15 @@
       <c r="AE71">
         <v>78.1632026851</v>
       </c>
+      <c r="AF71">
+        <v>95.82696878260001</v>
+      </c>
+      <c r="AG71">
+        <v>119.295739353</v>
+      </c>
+      <c r="AH71">
+        <v>141.0301472726</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72">
@@ -7258,6 +7903,15 @@
       <c r="AE72">
         <v>0</v>
       </c>
+      <c r="AF72">
+        <v>0</v>
+      </c>
+      <c r="AG72">
+        <v>0</v>
+      </c>
+      <c r="AH72">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73">
@@ -7353,6 +8007,15 @@
       <c r="AE73">
         <v>0</v>
       </c>
+      <c r="AF73">
+        <v>0</v>
+      </c>
+      <c r="AG73">
+        <v>0</v>
+      </c>
+      <c r="AH73">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74">
@@ -7448,6 +8111,15 @@
       <c r="AE74">
         <v>86.913658161</v>
       </c>
+      <c r="AF74">
+        <v>101.916427861</v>
+      </c>
+      <c r="AG74">
+        <v>107.917648646</v>
+      </c>
+      <c r="AH74">
+        <v>127.79899625</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75">
@@ -7543,6 +8215,15 @@
       <c r="AE75">
         <v>77.9781933</v>
       </c>
+      <c r="AF75">
+        <v>101.903279745</v>
+      </c>
+      <c r="AG75">
+        <v>123.107824233</v>
+      </c>
+      <c r="AH75">
+        <v>137.905860639</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76">
@@ -7638,6 +8319,15 @@
       <c r="AE76">
         <v>0</v>
       </c>
+      <c r="AF76">
+        <v>0</v>
+      </c>
+      <c r="AG76">
+        <v>0</v>
+      </c>
+      <c r="AH76">
+        <v>0</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77">
@@ -7733,6 +8423,15 @@
       <c r="AE77">
         <v>0</v>
       </c>
+      <c r="AF77">
+        <v>0</v>
+      </c>
+      <c r="AG77">
+        <v>0</v>
+      </c>
+      <c r="AH77">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78">
@@ -7827,6 +8526,15 @@
       </c>
       <c r="AE78">
         <v>80.57376613700001</v>
+      </c>
+      <c r="AF78">
+        <v>106.924648905</v>
+      </c>
+      <c r="AG78">
+        <v>138.208306918</v>
+      </c>
+      <c r="AH78">
+        <v>158.930296279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>